<commit_message>
Made way to see how checks change with different offsets
</commit_message>
<xml_diff>
--- a/data/Wetland_well_metadata_1.xlsx
+++ b/data/Wetland_well_metadata_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28521"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hydrology\Bradford_Forest_Project\Masterfiles_latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmaze/Documents/projects/doe_pt_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22D7E863-43AE-44B7-B831-D454DA68BA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93AEC34-981F-F245-BF43-27FAEAFF0BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="1080" windowWidth="16620" windowHeight="11295" tabRatio="698" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52280" yWindow="3260" windowWidth="27820" windowHeight="15780" tabRatio="698" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wetland_and_well_info" sheetId="9" r:id="rId1"/>
@@ -1177,7 +1177,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1339,9 +1339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1379,7 +1379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1485,7 +1485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1627,7 +1627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1641,26 +1641,26 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="12" style="15" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="79.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="5"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="79.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="5"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -1805,7 +1805,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1851,7 +1851,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -1897,7 +1897,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -1943,7 +1943,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -1983,7 +1983,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>51</v>
       </c>
@@ -2180,7 +2180,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>54</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="5" customFormat="1">
+    <row r="14" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>64</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>70</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>73</v>
       </c>
@@ -2480,7 +2480,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>78</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>80</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>90</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>93</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>99</v>
       </c>
@@ -2864,7 +2864,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>102</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>105</v>
       </c>
@@ -2950,7 +2950,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>108</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>111</v>
       </c>
@@ -3038,7 +3038,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="6"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>113</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>119</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>127</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>130</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>132</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="6"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>135</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="6"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>140</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>142</v>
       </c>
@@ -3460,7 +3460,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>145</v>
       </c>
@@ -3500,7 +3500,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>148</v>
       </c>
@@ -3540,7 +3540,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" s="13" customFormat="1">
+    <row r="46" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>150</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>152</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>154</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>158</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>161</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>163</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>165</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>168</v>
       </c>
@@ -3852,55 +3852,55 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="C64" s="8"/>
       <c r="N64"/>
     </row>
-    <row r="75" spans="14:14">
+    <row r="75" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N75"/>
     </row>
-    <row r="78" spans="14:14">
+    <row r="78" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N78"/>
     </row>
   </sheetData>
@@ -3917,25 +3917,25 @@
       <selection pane="topRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="12" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -4052,7 +4052,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -4090,7 +4090,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -4128,7 +4128,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -4204,7 +4204,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>21248091</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>10776660</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>10776675</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>21248087</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>51</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>54</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>21248117</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1">
+    <row r="14" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>21094855</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>10776648</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>64</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>10776671</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>10744668</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>70</v>
       </c>
@@ -4595,7 +4595,7 @@
       <c r="M18" s="4"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>73</v>
       </c>
@@ -4633,7 +4633,7 @@
       <c r="M19" s="4"/>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>21248116</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>78</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>21248115</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>80</v>
       </c>
@@ -4741,7 +4741,7 @@
       <c r="M22" s="4"/>
       <c r="N22" s="6"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
@@ -4783,7 +4783,7 @@
       </c>
       <c r="N23" s="6"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
@@ -4825,7 +4825,7 @@
       </c>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>90</v>
       </c>
@@ -4863,7 +4863,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>93</v>
       </c>
@@ -4901,7 +4901,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
@@ -4943,7 +4943,7 @@
       </c>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>99</v>
       </c>
@@ -4985,7 +4985,7 @@
       </c>
       <c r="N28" s="6"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>102</v>
       </c>
@@ -5023,7 +5023,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>105</v>
       </c>
@@ -5061,7 +5061,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>108</v>
       </c>
@@ -5099,7 +5099,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>111</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="M32" s="4"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>113</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>21248120</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>10776685</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>119</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>21248102</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>21248096</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>127</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>21248099</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>130</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>21248104</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>132</v>
       </c>
@@ -5385,7 +5385,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>135</v>
       </c>
@@ -5423,7 +5423,7 @@
       <c r="M40" s="4"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -5461,7 +5461,7 @@
       <c r="M41" s="4"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>140</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="M42" s="4"/>
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>142</v>
       </c>
@@ -5537,7 +5537,7 @@
       <c r="M43" s="4"/>
       <c r="N43" s="6"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>145</v>
       </c>
@@ -5575,7 +5575,7 @@
       <c r="M44" s="4"/>
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>148</v>
       </c>
@@ -5613,7 +5613,7 @@
       <c r="M45" s="4"/>
       <c r="N45" s="6"/>
     </row>
-    <row r="46" spans="1:14" s="13" customFormat="1">
+    <row r="46" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>150</v>
       </c>
@@ -5651,7 +5651,7 @@
       <c r="M46" s="4"/>
       <c r="N46" s="6"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>152</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>10776673</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>154</v>
       </c>
@@ -5724,7 +5724,7 @@
       <c r="M48" s="4"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>158</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>21248141</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>161</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>21248101</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>163</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>21248107</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>165</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>21248113</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>168</v>
       </c>
@@ -5905,50 +5905,50 @@
         <v>21248109</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="C54" s="8"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="C55" s="8"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="C56" s="8"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="C64" s="8"/>
     </row>
@@ -5966,39 +5966,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1:U1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="23" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="17.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -6140,7 +6139,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -6326,7 +6325,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -6388,7 +6387,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -6450,7 +6449,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -6512,7 +6511,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -6574,7 +6573,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>51</v>
       </c>
@@ -6760,7 +6759,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>54</v>
       </c>
@@ -6822,7 +6821,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="5" customFormat="1">
+    <row r="14" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -6884,7 +6883,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>64</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
@@ -7079,7 +7078,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>70</v>
       </c>
@@ -7141,7 +7140,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>73</v>
       </c>
@@ -7212,7 +7211,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
@@ -7274,7 +7273,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>78</v>
       </c>
@@ -7336,7 +7335,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>80</v>
       </c>
@@ -7398,7 +7397,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
@@ -7460,7 +7459,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
@@ -7522,7 +7521,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>90</v>
       </c>
@@ -7584,7 +7583,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>93</v>
       </c>
@@ -7646,7 +7645,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
@@ -7708,7 +7707,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>99</v>
       </c>
@@ -7770,7 +7769,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>102</v>
       </c>
@@ -7832,7 +7831,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>105</v>
       </c>
@@ -7894,7 +7893,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>108</v>
       </c>
@@ -7956,7 +7955,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>111</v>
       </c>
@@ -8027,7 +8026,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>113</v>
       </c>
@@ -8089,7 +8088,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>119</v>
       </c>
@@ -8213,7 +8212,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
@@ -8275,7 +8274,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>127</v>
       </c>
@@ -8337,7 +8336,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>130</v>
       </c>
@@ -8399,7 +8398,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>132</v>
       </c>
@@ -8461,7 +8460,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>135</v>
       </c>
@@ -8523,7 +8522,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>140</v>
       </c>
@@ -8647,7 +8646,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>142</v>
       </c>
@@ -8709,7 +8708,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>145</v>
       </c>
@@ -8771,7 +8770,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>148</v>
       </c>
@@ -8833,7 +8832,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="13" customFormat="1">
+    <row r="46" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>150</v>
       </c>
@@ -8895,7 +8894,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>152</v>
       </c>
@@ -8957,7 +8956,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>154</v>
       </c>
@@ -9019,7 +9018,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>158</v>
       </c>
@@ -9081,7 +9080,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>161</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>163</v>
       </c>
@@ -9205,7 +9204,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>165</v>
       </c>
@@ -9267,7 +9266,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>168</v>
       </c>
@@ -9329,50 +9328,50 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="C54" s="8"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="C55" s="8"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="C56" s="8"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="C64" s="8"/>
     </row>
@@ -9392,26 +9391,26 @@
       <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="12" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -9467,7 +9466,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -9514,7 +9513,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -9550,7 +9549,7 @@
       </c>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -9586,7 +9585,7 @@
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -9622,7 +9621,7 @@
       </c>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -9658,7 +9657,7 @@
       </c>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -9694,7 +9693,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -9735,7 +9734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -9776,7 +9775,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -9825,7 +9824,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
@@ -9866,7 +9865,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>51</v>
       </c>
@@ -9907,7 +9906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>54</v>
       </c>
@@ -9956,7 +9955,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:18" s="5" customFormat="1">
+    <row r="14" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -9997,7 +9996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -10038,7 +10037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>64</v>
       </c>
@@ -10079,7 +10078,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
@@ -10120,7 +10119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>70</v>
       </c>
@@ -10161,7 +10160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>73</v>
       </c>
@@ -10210,7 +10209,7 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
@@ -10251,7 +10250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>78</v>
       </c>
@@ -10300,7 +10299,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>80</v>
       </c>
@@ -10341,7 +10340,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
@@ -10382,7 +10381,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
@@ -10423,7 +10422,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>90</v>
       </c>
@@ -10464,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>93</v>
       </c>
@@ -10505,7 +10504,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
@@ -10546,7 +10545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>99</v>
       </c>
@@ -10587,7 +10586,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>102</v>
       </c>
@@ -10628,7 +10627,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>105</v>
       </c>
@@ -10669,7 +10668,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>108</v>
       </c>
@@ -10710,7 +10709,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>111</v>
       </c>
@@ -10746,7 +10745,7 @@
       </c>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>113</v>
       </c>
@@ -10787,7 +10786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>115</v>
       </c>
@@ -10828,7 +10827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>119</v>
       </c>
@@ -10877,7 +10876,7 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
@@ -10926,7 +10925,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>127</v>
       </c>
@@ -10975,7 +10974,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>130</v>
       </c>
@@ -11024,7 +11023,7 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>132</v>
       </c>
@@ -11065,7 +11064,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>135</v>
       </c>
@@ -11106,7 +11105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -11147,7 +11146,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>140</v>
       </c>
@@ -11188,7 +11187,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>142</v>
       </c>
@@ -11229,7 +11228,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>145</v>
       </c>
@@ -11270,7 +11269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>148</v>
       </c>
@@ -11311,7 +11310,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="13" customFormat="1">
+    <row r="46" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>150</v>
       </c>
@@ -11352,7 +11351,7 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>152</v>
       </c>
@@ -11393,7 +11392,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>154</v>
       </c>
@@ -11434,7 +11433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>158</v>
       </c>
@@ -11470,7 +11469,7 @@
       </c>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>161</v>
       </c>
@@ -11506,7 +11505,7 @@
       </c>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>163</v>
       </c>
@@ -11542,7 +11541,7 @@
       </c>
       <c r="L51"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>165</v>
       </c>
@@ -11578,7 +11577,7 @@
       </c>
       <c r="L52"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>168</v>
       </c>
@@ -11614,47 +11613,47 @@
       </c>
       <c r="L53"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="C64" s="8"/>
     </row>

</xml_diff>